<commit_message>
Forgot to push FlatWing
</commit_message>
<xml_diff>
--- a/HW4/theory comparison.xlsx
+++ b/HW4/theory comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eden\Documents\GitHub\AerodynamicsOfWingsAndBodies\HW4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49956579-BA20-4108-8768-A2562595BEC2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5577F082-A588-4EF6-8C6C-1E2F7FFA045B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18408" windowHeight="8772" xr2:uid="{CB66503A-5BD0-4AAD-B898-D871C27C8CDD}"/>
   </bookViews>
@@ -477,13 +477,13 @@
         <v>0.25</v>
       </c>
       <c r="D2">
-        <v>0.34507426290359644</v>
+        <v>0.38013691964065927</v>
       </c>
       <c r="E2">
-        <v>0.56289679150813887</v>
+        <v>0.54737570206066166</v>
       </c>
       <c r="F2">
-        <v>0.28641567053547545</v>
+        <v>0.31982659424771431</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -497,13 +497,13 @@
         <v>0.25</v>
       </c>
       <c r="D3">
-        <v>4.6027203054127976E-2</v>
+        <v>6.4075224142106035E-2</v>
       </c>
       <c r="E3">
-        <v>0.53604925260902747</v>
+        <v>0.53561436446007782</v>
       </c>
       <c r="F3">
-        <v>0.17832707673314196</v>
+        <v>0.19758996236955251</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -517,13 +517,13 @@
         <v>0.25</v>
       </c>
       <c r="D4">
-        <v>5.2951491181712391E-2</v>
+        <v>6.4511134667174883E-2</v>
       </c>
       <c r="E4">
-        <v>0.36027410021886719</v>
+        <v>0.36125841268767245</v>
       </c>
       <c r="F4">
-        <v>0.11941662492758454</v>
+        <v>0.13298607494057224</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -537,13 +537,13 @@
         <v>0.25</v>
       </c>
       <c r="D5">
-        <v>0.13083124824039083</v>
+        <v>0.13888180900026556</v>
       </c>
       <c r="E5">
-        <v>0.12018390545798403</v>
+        <v>0.12183814259614477</v>
       </c>
       <c r="F5">
-        <v>8.4749785420285662E-2</v>
+        <v>9.5159108012391469E-2</v>
       </c>
     </row>
   </sheetData>
@@ -595,13 +595,13 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D2">
-        <v>7.9850271875008094E-2</v>
+        <v>5.5864314405044503E-2</v>
       </c>
       <c r="E2">
-        <v>0.79544576612566065</v>
+        <v>0.78818225375800222</v>
       </c>
       <c r="F2">
-        <v>1.2616063895857788E-3</v>
+        <v>9.5273377258247027E-3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -615,13 +615,13 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D3">
-        <v>0.32821320556207834</v>
+        <v>0.31662228116045604</v>
       </c>
       <c r="E3">
-        <v>0.80864102072956023</v>
+        <v>0.8084616487752142</v>
       </c>
       <c r="F3">
-        <v>3.6165214804922796E-2</v>
+        <v>2.9944907984831848E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -635,13 +635,13 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D4">
-        <v>0.54013385606919129</v>
+        <v>0.53508529616933442</v>
       </c>
       <c r="E4">
-        <v>0.87797745451111198</v>
+        <v>0.87816520415989308</v>
       </c>
       <c r="F4">
-        <v>5.518838153380079E-2</v>
+        <v>5.0806579967106746E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -655,13 +655,13 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D5">
-        <v>0.68128346848172272</v>
+        <v>0.67901447670584369</v>
       </c>
       <c r="E5">
-        <v>0.93011153826874093</v>
+        <v>0.93024294310395828</v>
       </c>
       <c r="F5">
-        <v>6.6382881791366088E-2</v>
+        <v>6.3021538037665248E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>